<commit_message>
update db assertion login
</commit_message>
<xml_diff>
--- a/src/test/java/testCases/login/loginTestData.xlsx
+++ b/src/test/java/testCases/login/loginTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinwinarko/eclipse-workspace/DanaPulsaAutomationTest/src/test/java/testCases/login/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC0EF80-01DF-DC4D-B192-252FCE67EA22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622B3083-499C-E54B-BDC8-E21E72CA9DC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
   </bookViews>
@@ -33,12 +33,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>phone</t>
   </si>
   <si>
     <t>082164886204</t>
+  </si>
+  <si>
+    <t>abcdefghi</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>6282164886204</t>
+  </si>
+  <si>
+    <t>+6282164886204</t>
+  </si>
+  <si>
+    <t>08216488</t>
+  </si>
+  <si>
+    <t>08216488620444</t>
+  </si>
+  <si>
+    <t>082111112222</t>
   </si>
 </sst>
 </file>
@@ -77,7 +98,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -85,20 +106,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -414,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A09F2C92-1070-F549-ABD8-21E67EECDFEF}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -429,7 +468,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -437,18 +476,52 @@
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
+      <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="2"/>
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>